<commit_message>
Update 2022-2023-2 嵌入式原理及应用B  Course Arrangement 成绩评定表 物联网32131.xlsx
</commit_message>
<xml_diff>
--- a/2022-2023-2 嵌入式原理及应用B  Course Arrangement 成绩评定表 物联网32131.xlsx
+++ b/2022-2023-2 嵌入式原理及应用B  Course Arrangement 成绩评定表 物联网32131.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop-Lenovo\Qt Embedded嵌入式原理及应用\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yi Ping\Documents\GitHub\Qt-Embedded-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B691D0E3-B4AF-494F-935A-822A1DB5F775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA447A0E-BF2D-42F8-89BA-91D3BEC6A7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{56D46586-203F-4DA5-8833-0738A3BCF6C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{56D46586-203F-4DA5-8833-0738A3BCF6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Information 物联网92061" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="164">
   <si>
     <t>Student ID(学号)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -541,6 +541,10 @@
   </si>
   <si>
     <t>请假</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈非凡</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -548,7 +552,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,6 +736,27 @@
       <family val="3"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -803,7 +828,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -904,6 +929,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1965,7 +2002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91AC44C4-55D5-4851-BBF2-151A82E50550}">
   <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L3" sqref="L3:M48"/>
     </sheetView>
   </sheetViews>
@@ -5205,10 +5242,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06EBC456-0353-452F-B62B-0A1B41F55AD0}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5274,7 +5311,9 @@
       <c r="D3" s="30"/>
       <c r="E3" s="18"/>
       <c r="F3" s="16"/>
-      <c r="G3" s="18"/>
+      <c r="G3" s="18">
+        <v>87</v>
+      </c>
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5290,7 +5329,9 @@
       <c r="D4" s="30"/>
       <c r="E4" s="18"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="18"/>
+      <c r="G4" s="34">
+        <v>57</v>
+      </c>
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5306,7 +5347,9 @@
       <c r="D5" s="30"/>
       <c r="E5" s="18"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="34">
+        <v>57</v>
+      </c>
       <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5322,7 +5365,9 @@
       <c r="D6" s="30"/>
       <c r="E6" s="18"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="34">
+        <v>53</v>
+      </c>
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5338,7 +5383,9 @@
       <c r="D7" s="30"/>
       <c r="E7" s="18"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="18"/>
+      <c r="G7" s="18">
+        <v>87</v>
+      </c>
       <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5354,7 +5401,9 @@
       <c r="D8" s="30"/>
       <c r="E8" s="18"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="18">
+        <v>79</v>
+      </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5370,7 +5419,9 @@
       <c r="D9" s="30"/>
       <c r="E9" s="18"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="37">
+        <v>35</v>
+      </c>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5386,7 +5437,9 @@
       <c r="D10" s="30"/>
       <c r="E10" s="18"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="34">
+        <v>54</v>
+      </c>
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5402,7 +5455,9 @@
       <c r="D11" s="30"/>
       <c r="E11" s="18"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="18">
+        <v>82</v>
+      </c>
       <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5418,7 +5473,9 @@
       <c r="D12" s="30"/>
       <c r="E12" s="18"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="18">
+        <v>60</v>
+      </c>
       <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5434,7 +5491,9 @@
       <c r="D13" s="30"/>
       <c r="E13" s="18"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="18"/>
+      <c r="G13" s="18">
+        <v>63</v>
+      </c>
       <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5450,7 +5509,9 @@
       <c r="D14" s="30"/>
       <c r="E14" s="18"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="18">
+        <v>67</v>
+      </c>
       <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5466,7 +5527,9 @@
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
       <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="G15" s="35">
+        <v>54</v>
+      </c>
       <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5482,7 +5545,9 @@
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="G16" s="28">
+        <v>85</v>
+      </c>
       <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5498,7 +5563,9 @@
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="28">
+        <v>78</v>
+      </c>
       <c r="H17" s="29"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5514,7 +5581,9 @@
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
       <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="G18" s="28">
+        <v>68</v>
+      </c>
       <c r="H18" s="29"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5530,7 +5599,9 @@
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
       <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
+      <c r="G19" s="28">
+        <v>60</v>
+      </c>
       <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5546,7 +5617,9 @@
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
+      <c r="G20" s="35">
+        <v>46</v>
+      </c>
       <c r="H20" s="29"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5562,7 +5635,9 @@
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="G21" s="28">
+        <v>82</v>
+      </c>
       <c r="H21" s="29"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5578,7 +5653,9 @@
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
+      <c r="G22" s="35">
+        <v>56</v>
+      </c>
       <c r="H22" s="29"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5594,7 +5671,9 @@
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
+      <c r="G23" s="28">
+        <v>62</v>
+      </c>
       <c r="H23" s="29"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5610,7 +5689,9 @@
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="G24" s="28">
+        <v>78</v>
+      </c>
       <c r="H24" s="29"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5626,7 +5707,9 @@
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
+      <c r="G25" s="28">
+        <v>69</v>
+      </c>
       <c r="H25" s="29"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5642,7 +5725,9 @@
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
+      <c r="G26" s="28">
+        <v>85</v>
+      </c>
       <c r="H26" s="29"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5658,7 +5743,9 @@
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
       <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
+      <c r="G27" s="28">
+        <v>72</v>
+      </c>
       <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5674,7 +5761,9 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
+      <c r="G28" s="35">
+        <v>48</v>
+      </c>
       <c r="H28" s="29"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5690,7 +5779,9 @@
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
+      <c r="G29" s="28">
+        <v>74</v>
+      </c>
       <c r="H29" s="29"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5706,7 +5797,9 @@
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="G30" s="28">
+        <v>92</v>
+      </c>
       <c r="H30" s="29"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5722,7 +5815,9 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="28">
+        <v>77</v>
+      </c>
       <c r="H31" s="29"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5738,7 +5833,9 @@
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
+      <c r="G32" s="35">
+        <v>55</v>
+      </c>
       <c r="H32" s="29"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5754,7 +5851,9 @@
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="G33" s="28">
+        <v>76</v>
+      </c>
       <c r="H33" s="29"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5770,7 +5869,9 @@
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
+      <c r="G34" s="28">
+        <v>69</v>
+      </c>
       <c r="H34" s="29"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5786,7 +5887,9 @@
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
+      <c r="G35" s="35">
+        <v>57</v>
+      </c>
       <c r="H35" s="29"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5802,7 +5905,9 @@
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
       <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
+      <c r="G36" s="28">
+        <v>61</v>
+      </c>
       <c r="H36" s="29"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5818,7 +5923,9 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
+      <c r="G37" s="28">
+        <v>64</v>
+      </c>
       <c r="H37" s="29"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5834,7 +5941,9 @@
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
+      <c r="G38" s="35">
+        <v>59</v>
+      </c>
       <c r="H38" s="29"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5850,7 +5959,9 @@
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
       <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
+      <c r="G39" s="28">
+        <v>73</v>
+      </c>
       <c r="H39" s="29"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5866,7 +5977,9 @@
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
       <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
+      <c r="G40" s="28">
+        <v>73</v>
+      </c>
       <c r="H40" s="29"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5882,7 +5995,9 @@
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
+      <c r="G41" s="28">
+        <v>64</v>
+      </c>
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5898,7 +6013,9 @@
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
+      <c r="G42" s="35">
+        <v>51</v>
+      </c>
       <c r="H42" s="29"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5914,7 +6031,9 @@
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
+      <c r="G43" s="28">
+        <v>71</v>
+      </c>
       <c r="H43" s="29"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5930,7 +6049,9 @@
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
+      <c r="G44" s="28">
+        <v>63</v>
+      </c>
       <c r="H44" s="29"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5946,7 +6067,9 @@
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
+      <c r="G45" s="28">
+        <v>61</v>
+      </c>
       <c r="H45" s="29"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5962,7 +6085,9 @@
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
       <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
+      <c r="G46" s="28">
+        <v>78</v>
+      </c>
       <c r="H46" s="29"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5978,7 +6103,9 @@
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
       <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
+      <c r="G47" s="28">
+        <v>70</v>
+      </c>
       <c r="H47" s="29"/>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5994,8 +6121,28 @@
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
       <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="G48" s="35">
+        <v>46</v>
+      </c>
       <c r="H48" s="29"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="26">
+        <v>3040193302</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28">
+        <v>64</v>
+      </c>
+      <c r="H49" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6008,6 +6155,66 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Invited_Students xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <FolderType xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <CultureName xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Student_Groups xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <DefaultSectionNames xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Templates xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <NotebookType xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Teachers xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Invited_Teachers xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Math_Settings xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Owner xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Distribution_Groups xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <AppVersion xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <LMS_Mappings xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033F188CDD829674AAD05B93C069E2813" ma:contentTypeVersion="25" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12f87a5caa000e69b2f4c8c0b3e42f66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="773ac416-4a36-402f-a3b6-d25dea329997" xmlns:ns4="63d2042b-7b91-46d4-baa3-a67d3669a720" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f06fb7f16fd173aa8b0bb68049ad5879" ns3:_="" ns4:_="">
     <xsd:import namespace="773ac416-4a36-402f-a3b6-d25dea329997"/>
@@ -6366,81 +6573,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Invited_Students xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <FolderType xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <CultureName xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Student_Groups xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <DefaultSectionNames xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Templates xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <NotebookType xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Teachers xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Invited_Teachers xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Math_Settings xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Owner xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Distribution_Groups xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <AppVersion xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <LMS_Mappings xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="63d2042b-7b91-46d4-baa3-a67d3669a720" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6741670B-461B-4661-A53C-BD46BBECF45E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AFF0ECA-8F3D-4871-93DE-8F766A9E7256}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="773ac416-4a36-402f-a3b6-d25dea329997"/>
-    <ds:schemaRef ds:uri="63d2042b-7b91-46d4-baa3-a67d3669a720"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6463,9 +6599,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AFF0ECA-8F3D-4871-93DE-8F766A9E7256}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6741670B-461B-4661-A53C-BD46BBECF45E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="773ac416-4a36-402f-a3b6-d25dea329997"/>
+    <ds:schemaRef ds:uri="63d2042b-7b91-46d4-baa3-a67d3669a720"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>